<commit_message>
Corrección en las solicitudes
Cambio en el nombre de los archivos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/LE_06_08_REC220_Solicitud_Grafica.xlsx
+++ b/fuentes/contenidos/grado06/guion08/LE_06_08_REC220_Solicitud_Grafica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cris\Documents\GitHub\Lenguaje\fuentes\contenidos\grado06\guion08\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="197">
   <si>
     <t>Fecha:</t>
   </si>
@@ -604,40 +604,25 @@
     <t>Cristian Pineda</t>
   </si>
   <si>
+    <t>Personas de diferentes oficios y profesiones</t>
+  </si>
+  <si>
+    <t>Bombero apagando fuego</t>
+  </si>
+  <si>
+    <t>Mujer afrodescendiente con vestido tradicional</t>
+  </si>
+  <si>
+    <t>Monje leyendo un libro</t>
+  </si>
+  <si>
+    <t>Mujer trabajadora en una fábrica</t>
+  </si>
+  <si>
+    <t>Piloto al volante</t>
+  </si>
+  <si>
     <t>LE_06_08_REC220</t>
-  </si>
-  <si>
-    <t>Jóvenes raperos bailando</t>
-  </si>
-  <si>
-    <t>Joven haciendo un grafiti</t>
-  </si>
-  <si>
-    <t>Hombre montando en patineta</t>
-  </si>
-  <si>
-    <t>Joven hipster con bigote</t>
-  </si>
-  <si>
-    <t>Chica altenativa</t>
-  </si>
-  <si>
-    <t>Hombre tocando guitarra eléctrica</t>
-  </si>
-  <si>
-    <t>Ubicar en la sección "Definición"</t>
-  </si>
-  <si>
-    <t>Ubicar en la sección "Indumentaria"</t>
-  </si>
-  <si>
-    <t>Ubicar en la sección "Practica"</t>
-  </si>
-  <si>
-    <t>Brake dancers</t>
-  </si>
-  <si>
-    <t>Ubicar en laficha 2, "grupos urbanos", de la sección "Indumentaria"</t>
   </si>
 </sst>
 </file>
@@ -2515,7 +2500,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2553,7 +2538,7 @@
       </c>
       <c r="M1" s="2" t="str">
         <f>CONCATENATE('Definición técnica de imagenes'!$B$1," ",$G$5)</f>
-        <v>Ubicación de la imagen en el recurso F6</v>
+        <v>Ubicación de la imagen en el recurso F7</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -2664,8 +2649,8 @@
         <f>IF(G4="Recurso","Motor del recurso","")</f>
         <v>Motor del recurso</v>
       </c>
-      <c r="G5" s="71" t="s">
-        <v>132</v>
+      <c r="G5" s="61" t="s">
+        <v>135</v>
       </c>
       <c r="H5" s="58"/>
       <c r="I5" s="58"/>
@@ -2713,7 +2698,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -2778,7 +2763,7 @@
       </c>
       <c r="E9" s="18" t="str">
         <f>IF($G$4="Recurso",$M$1,$L$1)</f>
-        <v>Ubicación de la imagen en el recurso F6</v>
+        <v>Ubicación de la imagen en el recurso F7</v>
       </c>
       <c r="F9" s="57" t="s">
         <v>61</v>
@@ -2803,17 +2788,17 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
       <c r="B10" s="62">
-        <v>149212100</v>
+        <v>111119858</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
-        <v>Recurso F6</v>
+        <v>Recurso F7</v>
       </c>
       <c r="D10" s="63" t="s">
         <v>187</v>
@@ -2838,7 +2823,7 @@
         <v/>
       </c>
       <c r="J10" s="63" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
@@ -2852,11 +2837,11 @@
         <v>IMG02</v>
       </c>
       <c r="B11" s="62">
-        <v>295507979</v>
+        <v>282060272</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F6</v>
+        <v>Recurso F7</v>
       </c>
       <c r="D11" s="63" t="s">
         <v>187</v>
@@ -2881,7 +2866,7 @@
         <v/>
       </c>
       <c r="J11" s="64" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K11" s="64"/>
       <c r="O11" s="2" t="str">
@@ -2895,11 +2880,11 @@
         <v>IMG03</v>
       </c>
       <c r="B12" s="62">
-        <v>143687476</v>
+        <v>300290276</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F6</v>
+        <v>Recurso F7</v>
       </c>
       <c r="D12" s="63" t="s">
         <v>187</v>
@@ -2932,17 +2917,17 @@
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
       <c r="B13" s="62">
-        <v>156481154</v>
+        <v>269627873</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F6</v>
+        <v>Recurso F7</v>
       </c>
       <c r="D13" s="63" t="s">
         <v>187</v>
@@ -2967,27 +2952,25 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>194</v>
-      </c>
-      <c r="K13" s="64" t="s">
-        <v>197</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="K13" s="64"/>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
         <v>F4</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG05</v>
       </c>
       <c r="B14" s="62">
-        <v>176264750</v>
+        <v>361652273</v>
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F6</v>
+        <v>Recurso F7</v>
       </c>
       <c r="D14" s="63" t="s">
         <v>187</v>
@@ -3012,11 +2995,9 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J14" s="64" t="s">
-        <v>195</v>
-      </c>
-      <c r="K14" s="64" t="s">
-        <v>198</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="K14" s="64"/>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
         <v>F6</v>
@@ -3028,11 +3009,11 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="62">
-        <v>69214087</v>
+        <v>162914456</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F6</v>
+        <v>Recurso F7</v>
       </c>
       <c r="D15" s="63" t="s">
         <v>187</v>
@@ -3057,56 +3038,44 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="K15" s="64" t="s">
-        <v>199</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
       </c>
     </row>
-    <row r="16" spans="1:16" s="11" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" s="11" customFormat="1" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>IMG07</v>
-      </c>
-      <c r="B16" s="62">
-        <v>241825993</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B16" s="62"/>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>Recurso F6</v>
-      </c>
-      <c r="D16" s="63" t="s">
-        <v>187</v>
-      </c>
-      <c r="E16" s="63" t="s">
-        <v>155</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D16" s="63"/>
+      <c r="E16" s="63"/>
       <c r="F16" s="13" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>LE_06_08_REC220_IMG07n.jpg</v>
+        <f t="shared" si="4"/>
+        <v/>
       </c>
       <c r="G16" s="13" t="str">
         <f ca="1">IF($F16&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>320 x 480 px</v>
+        <v/>
       </c>
       <c r="H16" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>LE_06_08_REC220_IMG07a.jpg</v>
+        <v/>
       </c>
       <c r="I16" s="13" t="str">
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
-        <v>800 x 458 px</v>
-      </c>
-      <c r="J16" s="67" t="s">
-        <v>200</v>
-      </c>
-      <c r="K16" s="68" t="s">
-        <v>201</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J16" s="67"/>
+      <c r="K16" s="68"/>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
         <v>F7</v>

</xml_diff>